<commit_message>
clean up of the repo
</commit_message>
<xml_diff>
--- a/03_analysis/child_academic_count.xlsx
+++ b/03_analysis/child_academic_count.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romanxaver/Desktop/DIS18_foerstner_projektarbeit1/dis18_graph_analysis/03_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{55B34C82-8EFA-0F45-8501-659C079A8604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F5F66834-4A44-DF44-9E2B-38D5C4DCD099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Pivot" sheetId="3" r:id="rId2"/>
-    <sheet name="test" sheetId="5" r:id="rId3"/>
+    <sheet name="visualization" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$F$2342</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">test!$B$2:$C$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">visualization!$B$2:$C$31</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">Pivot!$E$59:$E$87</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Pivot!$F$59:$F$87</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Pivot!$E$59:$E$87</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Pivot!$F$59:$F$87</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">test!$B$2</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">test!$B$3:$B$31</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">test!$C$2</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">test!$C$3:$C$31</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">visualization!$B$2</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">visualization!$B$3:$B$31</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">visualization!$C$2</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">visualization!$C$3:$C$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -12965,7 +12965,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13145,6 +13145,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -13307,14 +13313,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="33" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -13429,7 +13436,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>test!$C$2</c:f>
+              <c:f>visualization!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -13464,7 +13471,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>test!$B$3:$B$31</c:f>
+              <c:f>visualization!$B$3:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -13560,7 +13567,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>test!$C$3:$C$31</c:f>
+              <c:f>visualization!$C$3:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -13897,7 +13904,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>test!$C$2</c:f>
+              <c:f>visualization!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -13918,7 +13925,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>test!$B$3:$B$31</c:f>
+              <c:f>visualization!$B$3:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -14014,7 +14021,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>test!$C$3:$C$31</c:f>
+              <c:f>visualization!$C$3:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -15383,15 +15390,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>50800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15419,13 +15426,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -25594,7 +25601,7 @@
   <dimension ref="A1:F2342"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F2335"/>
+      <selection activeCell="H224" sqref="H224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -72455,8 +72462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F88"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59:F87"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -73338,7 +73345,7 @@
   <dimension ref="B2:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -73590,10 +73597,10 @@
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>4256</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="5">
         <f>_xlfn.RRI(E3,C3,C31)</f>
         <v>2.1351917874972814E-2</v>
       </c>

</xml_diff>